<commit_message>
plan de tests bien avancé
</commit_message>
<xml_diff>
--- a/testsUnitaires.xlsx
+++ b/testsUnitaires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmcob/Documents/Travail/websites/jmax.dev/kanap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D67526D4-2490-9E43-A5C7-BF26821A7FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{610BC9AC-5176-814A-B6B3-E793C92856FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="10800" xr2:uid="{ED51B0A2-C6B6-F447-A0DD-BA05B3CFD5D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="8780" xr2:uid="{ED51B0A2-C6B6-F447-A0DD-BA05B3CFD5D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="88">
   <si>
     <t>Lignes de code testées</t>
   </si>
@@ -103,13 +103,199 @@
     <t>qtyValue()</t>
   </si>
   <si>
-    <t>récupère la vaeur du champ quatité sur la page product</t>
-  </si>
-  <si>
     <t>au bouton ajouter au panier, il se retrouve dans le localStorage</t>
   </si>
   <si>
     <t>ajout a zero ou si la couleur n'a pas été choisie doit etre évitée</t>
+  </si>
+  <si>
+    <t>50 à 53</t>
+  </si>
+  <si>
+    <t>colorValue()</t>
+  </si>
+  <si>
+    <t>récupère la valeur du champ "couleur" sur la page product afin d'etre après ajoutée au localStorage</t>
+  </si>
+  <si>
+    <t>récupère la valeur du champ "quantité" sur la page product afin d'etre après ajoutée au localStorage</t>
+  </si>
+  <si>
+    <t>si "aucune couleur selectionnée" devrait ne pas fonctionner, mais peut etre un probleme</t>
+  </si>
+  <si>
+    <t>58 à 62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toCartBtn.addEventListener("click", () </t>
+  </si>
+  <si>
+    <t>récupère les valeurs de "qtyValue() et colorValue()" et les envoie a la fction add2cart() de la page cart.js avec l'id du produit définie dans les 3 premieres lignes de product.js</t>
+  </si>
+  <si>
+    <t>au bouton ajouter au panier, id, color et qty se retrouvent dans le localStorage</t>
+  </si>
+  <si>
+    <t>si une des trois valeur, "id, color ou qty" est nulle cela devrait etre incomplet dans le localStorage</t>
+  </si>
+  <si>
+    <t>cart.js</t>
+  </si>
+  <si>
+    <t>6 à 12</t>
+  </si>
+  <si>
+    <t>getCart()</t>
+  </si>
+  <si>
+    <t>récupère la valeur "panier" du localStorage dans une variable items qui est la sortie de la fonction</t>
+  </si>
+  <si>
+    <t>utilisé dans plusieurs fonctions, la fonction getCart permet de stocker dans une variable le localStorage, notamment dans "add2cart(), deleteItem(), changeQuantity(), fetchIdData(), makeJsonData()". Cette variable est tout le temps items donc il suffit de surveiller items dans l'inspecteur</t>
+  </si>
+  <si>
+    <t>si le panier dans le localStorage n'est pas complet, items ne sera pas complet et tout bug. Mais cette fonction tres utilisée est essentielle a d'autres fonctions donc les bugs peuvent etre multiple si elle ne fonctionne pas</t>
+  </si>
+  <si>
+    <t>15 à 36</t>
+  </si>
+  <si>
+    <t>add2cart()</t>
+  </si>
+  <si>
+    <t>construit le panier du localStorage, prend en compte le panier existant</t>
+  </si>
+  <si>
+    <t>regarder le localStorage</t>
+  </si>
+  <si>
+    <t>definitions de items par getCart() mauvaise ; ou envoie de "id, color et qty"par "toCartBtn.addEventListener("click", () " dans la page product mauvais aussi.</t>
+  </si>
+  <si>
+    <t>deleteItem()</t>
+  </si>
+  <si>
+    <t>supprime une entrée du panier de html et du localStorage, et reload la page</t>
+  </si>
+  <si>
+    <t>l'entrée html doit etre supprimée et l'entrée localStorage doit être supprimée</t>
+  </si>
+  <si>
+    <t>39 à 52</t>
+  </si>
+  <si>
+    <t>54 à 63</t>
+  </si>
+  <si>
+    <t>la page pourrait ne pas se recharger, et l'html ne pas effacer la zone du kanap a supprimer. "splice()" pourrait rendre un mauvais "items" et dans ce cas corrompre le nouveau panier</t>
+  </si>
+  <si>
+    <t>modifie la quantité d'un item demandé par l'utilisateur dans le local storage.</t>
+  </si>
+  <si>
+    <t>Lorsque on modifie la quantité d'un kanap dans la panier, le localstorage doit etre immediatement modifié pour la valeur du client.</t>
+  </si>
+  <si>
+    <t>Si "getCart()" est corrompu la suite est corrompue. Si le panier ne correspond pas au localstorage, le changement ne se fera pas</t>
+  </si>
+  <si>
+    <t>71 à 118</t>
+  </si>
+  <si>
+    <t>fetchIdData()</t>
+  </si>
+  <si>
+    <t>changeQuantity()</t>
+  </si>
+  <si>
+    <t>affiche en innerHTML les éléments du panier et leur contenu de l'API. Affiche panier vide si panier vide.</t>
+  </si>
+  <si>
+    <t>les éléménets s'affichent correctement et completement : l'image, son texte alt, le nom du kanap, sa couleur, son prix, sa quantité désirée, son prix total, le nombre d'articles total</t>
+  </si>
+  <si>
+    <t>Vérifier que le prix total et le nombre total d'article soit le bon. Problemes de fetch de l'API, si le back end n'est pas allumé par exemple. "getCart()" peut etre corrompu. La panier pourrait ne pas s'afficher comme vide en HTML dans le cas ou localStorage est null</t>
+  </si>
+  <si>
+    <t>133 à 142</t>
+  </si>
+  <si>
+    <t>validateEmail(mai)</t>
+  </si>
+  <si>
+    <t>Fonction REGEX pour valider une adresse email</t>
+  </si>
+  <si>
+    <t>si l'utilisateur entre une adresse non conforme, cette fonction affiche false. True pour l'inverse. Elle est declenchée par "orderButton.addEventListener("click", (e) =&gt;"</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer de mauvaises adresses mail.</t>
+  </si>
+  <si>
+    <t>validateFirstName(prenom)</t>
+  </si>
+  <si>
+    <t>validateLastName(nom)</t>
+  </si>
+  <si>
+    <t>validateCity(ville)</t>
+  </si>
+  <si>
+    <t>validateAddress(adresse)</t>
+  </si>
+  <si>
+    <t>147 à 154</t>
+  </si>
+  <si>
+    <t>Fonction regex pour valider un prenom sans chiffre</t>
+  </si>
+  <si>
+    <t>Fonction regex pour valider une adresse non vide</t>
+  </si>
+  <si>
+    <t>Fonction regex pour valider un nom sans chiffre</t>
+  </si>
+  <si>
+    <t>Fonction regex pour valider une ville sans chiffre</t>
+  </si>
+  <si>
+    <t>cette fonction ne doit laisser passer aucun chiffre</t>
+  </si>
+  <si>
+    <t>cette fonction demande au champ d'etre non-vide</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer des prenoms invalides</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer des noms invalides</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer des villes invalides</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer des champs vides</t>
+  </si>
+  <si>
+    <t>158 à 165</t>
+  </si>
+  <si>
+    <t>169 à 176</t>
+  </si>
+  <si>
+    <t>181 à 188</t>
+  </si>
+  <si>
+    <t>208 à 231</t>
+  </si>
+  <si>
+    <t>makeJsonData()</t>
+  </si>
+  <si>
+    <t>orderButton.addEventListener("click", (e) =&gt;</t>
+  </si>
+  <si>
+    <t>235 à 285</t>
   </si>
 </sst>
 </file>
@@ -492,10 +678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D31CD72-805B-E649-B635-AAFD42782361}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -597,13 +783,275 @@
         <v>22</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="1" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
plan de tests unitaires
</commit_message>
<xml_diff>
--- a/testsUnitaires.xlsx
+++ b/testsUnitaires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmcob/Documents/Travail/websites/jmax.dev/kanap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B3AE6CA-8D46-A044-9315-B9F4C09FF212}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE24DE1C-D048-C74E-B348-AD6DF696183C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28800" yWindow="-7420" windowWidth="38400" windowHeight="21600" xr2:uid="{ED51B0A2-C6B6-F447-A0DD-BA05B3CFD5D6}"/>
   </bookViews>
@@ -148,9 +148,6 @@
     <t>deleteItem()</t>
   </si>
   <si>
-    <t>supprime une entrée du panier de html et du localStorage, et reload la page</t>
-  </si>
-  <si>
     <t>l'entrée html doit etre supprimée et l'entrée localStorage doit être supprimée</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>affiche en innerHTML les éléments du panier et leur contenu de l'API. Affiche panier vide si panier vide.</t>
   </si>
   <si>
-    <t>les éléménets s'affichent correctement et completement : l'image, son texte alt, le nom du kanap, sa couleur, son prix, sa quantité désirée, son prix total, le nombre d'articles total</t>
-  </si>
-  <si>
     <t>133 à 142</t>
   </si>
   <si>
@@ -314,6 +308,12 @@
   </si>
   <si>
     <t>si ajout de "0" kanaps en quantité, pas d'ajout dans le local storage / ou si la couleur n'a pas été sélectionnée : pas d'ajout dans le localstorage</t>
+  </si>
+  <si>
+    <t>les éléments s'affichent correctement et completement : l'image, son texte alt, le nom du kanap, sa couleur, son prix, sa quantité désirée, son prix total, le nombre d'articles total</t>
+  </si>
+  <si>
+    <t>supprime une entrée du panier de html et du localStorage, et recharge la page</t>
   </si>
 </sst>
 </file>
@@ -698,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D31CD72-805B-E649-B635-AAFD42782361}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -708,7 +708,7 @@
     <col min="2" max="2" width="27.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="32.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="115.83203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="75.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="106.6640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="147.5" style="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -750,7 +750,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,7 +767,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -787,7 +787,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -807,7 +807,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -827,7 +827,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -847,7 +847,7 @@
         <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,10 +884,10 @@
         <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -895,19 +895,19 @@
         <v>29</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -915,19 +915,19 @@
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -935,19 +935,19 @@
         <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -955,19 +955,19 @@
         <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="F13" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -975,19 +975,19 @@
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -995,19 +995,19 @@
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>64</v>
-      </c>
       <c r="F15" s="1" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1015,19 +1015,19 @@
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1035,19 +1035,19 @@
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1055,19 +1055,19 @@
         <v>29</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1075,19 +1075,19 @@
         <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
mise a jour plans de tests unitaire
</commit_message>
<xml_diff>
--- a/testsUnitaires.xlsx
+++ b/testsUnitaires.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmcob/Documents/Travail/websites/jmax.dev/kanap/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE24DE1C-D048-C74E-B348-AD6DF696183C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27652CE5-C157-8346-BA1A-180F372E9243}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-7420" windowWidth="38400" windowHeight="21600" xr2:uid="{ED51B0A2-C6B6-F447-A0DD-BA05B3CFD5D6}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{ED51B0A2-C6B6-F447-A0DD-BA05B3CFD5D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="95">
   <si>
     <t>Lignes de code testées</t>
   </si>
@@ -166,9 +166,6 @@
     <t>Lorsque on modifie la quantité d'un kanap dans la panier, le localstorage doit etre immediatement modifié pour la valeur du client.</t>
   </si>
   <si>
-    <t>71 à 118</t>
-  </si>
-  <si>
     <t>fetchIdData()</t>
   </si>
   <si>
@@ -178,21 +175,12 @@
     <t>affiche en innerHTML les éléments du panier et leur contenu de l'API. Affiche panier vide si panier vide.</t>
   </si>
   <si>
-    <t>133 à 142</t>
-  </si>
-  <si>
-    <t>validateEmail(mai)</t>
-  </si>
-  <si>
     <t>Fonction REGEX pour valider une adresse email</t>
   </si>
   <si>
     <t>si l'utilisateur entre une adresse non conforme, cette fonction affiche false. True pour l'inverse. Elle est declenchée par "orderButton.addEventListener("click", (e) =&gt;"</t>
   </si>
   <si>
-    <t>la regex pourrait laisser passer de mauvaises adresses mail.</t>
-  </si>
-  <si>
     <t>validateFirstName(prenom)</t>
   </si>
   <si>
@@ -205,9 +193,6 @@
     <t>validateAddress(adresse)</t>
   </si>
   <si>
-    <t>147 à 154</t>
-  </si>
-  <si>
     <t>Fonction regex pour valider un prenom sans chiffre</t>
   </si>
   <si>
@@ -226,27 +211,6 @@
     <t>cette fonction demande au champ d'etre non-vide</t>
   </si>
   <si>
-    <t>la regex pourrait laisser passer des prenoms invalides</t>
-  </si>
-  <si>
-    <t>la regex pourrait laisser passer des noms invalides</t>
-  </si>
-  <si>
-    <t>la regex pourrait laisser passer des villes invalides</t>
-  </si>
-  <si>
-    <t>la regex pourrait laisser passer des champs vides</t>
-  </si>
-  <si>
-    <t>158 à 165</t>
-  </si>
-  <si>
-    <t>169 à 176</t>
-  </si>
-  <si>
-    <t>181 à 188</t>
-  </si>
-  <si>
     <t>makeJsonData()</t>
   </si>
   <si>
@@ -256,15 +220,9 @@
     <t>définition du json a envoyer a l'API : "contact" et "products" y sont inclus</t>
   </si>
   <si>
-    <t>234 à 284</t>
-  </si>
-  <si>
     <t>lors de l'envoi, si la réponse est de 200, le json a été accepté par l'API. Aussi verifiable dans l'onglet reseau de l'inspecteur sur la ligne correpondant au fetch "post"</t>
   </si>
   <si>
-    <t>208 à 228</t>
-  </si>
-  <si>
     <t>on passe a la page confirmation avec le numero de l'orderId affiché</t>
   </si>
   <si>
@@ -280,18 +238,9 @@
     <t>Non chargement du fichier objet json, cause probable : serveur backend non démarré</t>
   </si>
   <si>
-    <t>si aucune couleur n'est selectionnée</t>
-  </si>
-  <si>
     <t>il faut aller regarder le localStorage dans l'inspecteur</t>
   </si>
   <si>
-    <t>getCart() pourrait etre corrompu, ou la variable products, ou la variable contacts. Il pourrait y avoir des doublons dans products</t>
-  </si>
-  <si>
-    <t>les regex peuvent ne pas etre validées ; le json peut ne pas etre accepté par l'API (400); erreur réseau</t>
-  </si>
-  <si>
     <t>si une des trois valeur, "id, color ou qty" est null, le local storage peut etre corrompu</t>
   </si>
   <si>
@@ -301,19 +250,73 @@
     <t>definitions de la variable items par getCart() doit être mauvaise ; ou envoie de "id, color et qty"par la fonction "toCartBtn.addEventListener("click", () " dans la page product.html doit etre mauvais aussi.</t>
   </si>
   <si>
-    <t>Si "getCart()" est corrompu la suite est corrompue. Si le panier ne correspond pas au localstorage, le changement ne peut pas être bon</t>
-  </si>
-  <si>
     <t>Vérifier que le prix total et le nombre total d'article soit le bon. Problemes de fetch de l'API, si le serveur back end n'est pas démarré par exemple. "getCart()" peut etre corrompu. La panier pourrait ne pas s'afficher comme vide dans l'affichage du navigateur dans le cas ou localStorage est null</t>
   </si>
   <si>
-    <t>si ajout de "0" kanaps en quantité, pas d'ajout dans le local storage / ou si la couleur n'a pas été sélectionnée : pas d'ajout dans le localstorage</t>
-  </si>
-  <si>
     <t>les éléments s'affichent correctement et completement : l'image, son texte alt, le nom du kanap, sa couleur, son prix, sa quantité désirée, son prix total, le nombre d'articles total</t>
   </si>
   <si>
     <t>supprime une entrée du panier de html et du localStorage, et recharge la page</t>
+  </si>
+  <si>
+    <t>cartFetch.js</t>
+  </si>
+  <si>
+    <t>8 à 55</t>
+  </si>
+  <si>
+    <t>60 à 110</t>
+  </si>
+  <si>
+    <t>validateEmail(mail)</t>
+  </si>
+  <si>
+    <t>74 à 83</t>
+  </si>
+  <si>
+    <t>88 à 95</t>
+  </si>
+  <si>
+    <t>99 à 106</t>
+  </si>
+  <si>
+    <t>110 à 117</t>
+  </si>
+  <si>
+    <t>122 à 129</t>
+  </si>
+  <si>
+    <t>149 à 170</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer des prenoms invalides. La regex n'admet pas les chiffres, il faut les tester</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer des noms invalides. La regex n'admet pas les chiffres,  il faut les tester</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer des villes invalides. La regex n'admet pas les chiffres, il faut les tester.</t>
+  </si>
+  <si>
+    <t>les regex peuvent ne pas etre validées dans ce cas la le chargement de confirmation.html ne devrait pas se faire.; le json peut ne pas etre accepté par l'API (400), il faut verifier le json dans l'inspecteur qu'il corresponde a la definition lignes 131 à 146 de cart.js; erreur réseau</t>
+  </si>
+  <si>
+    <t>getCart() pourrait etre corrompu, ou la variable products, ou la variable contact, products et contacts sont definis lignes 131 à 146 de cart.js. Il pourrait y avoir des doublons dans products. Il faut tester en ajoutant des canapés de meme nom et de couleurs différentes au panier</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer des champs vides, il faut tester le champ vide.</t>
+  </si>
+  <si>
+    <t>la regex pourrait laisser passer de mauvaises adresses mail. La regex actuelle teste le champ sur le modele [xxx]@[xx].[xx] avec les caracetères admis dans les adresses mail</t>
+  </si>
+  <si>
+    <t>Si "getCart()" est corrompu la suite est corrompue il faut tester getCart dans les autres fonction pour confirmer, comme add2cart(). Si le panier ne correspond pas au localstorage, le changement ne peut pas être bon</t>
+  </si>
+  <si>
+    <t>si ajout de "0" kanaps en quantité, il ne doit pas y avoir d'ajout dans le local storage / ou si la couleur n'a pas été sélectionnée : pas d'ajout dans le localstorage</t>
+  </si>
+  <si>
+    <t>si aucune couleur n'est selectionnée, il ne doit pas y avoir d'ajout dans le localStorage</t>
   </si>
 </sst>
 </file>
@@ -698,8 +701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D31CD72-805B-E649-B635-AAFD42782361}">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -750,7 +753,7 @@
         <v>10</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,7 +770,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -787,7 +790,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -807,7 +810,7 @@
         <v>20</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -827,7 +830,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -847,7 +850,7 @@
         <v>28</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -867,7 +870,7 @@
         <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -884,10 +887,10 @@
         <v>36</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -901,7 +904,7 @@
         <v>37</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>93</v>
+        <v>74</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>38</v>
@@ -918,7 +921,7 @@
         <v>40</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>42</v>
@@ -927,7 +930,7 @@
         <v>43</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -935,19 +938,19 @@
         <v>29</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>44</v>
+        <v>79</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>92</v>
+        <v>48</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -955,19 +958,19 @@
         <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>49</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -975,19 +978,19 @@
         <v>29</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>62</v>
-      </c>
       <c r="F14" s="1" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -995,19 +998,19 @@
         <v>29</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1015,19 +1018,19 @@
         <v>29</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1035,59 +1038,59 @@
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F18" s="1" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>29</v>
+        <v>75</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>72</v>
+        <v>60</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>